<commit_message>
[Upd] Add blank cell to the tests.
</commit_message>
<xml_diff>
--- a/s-pipes-modules/module-tabular/src/test/resources/examples/mergedCells/input.xlsx
+++ b/s-pipes-modules/module-tabular/src/test/resources/examples/mergedCells/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\ctu-fee\kbss\s-pipes\s-pipes-modules\module-tabular\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\ctu-fee\kbss\s-pipes\s-pipes-modules\module-tabular\src\test\resources\examples\mergedCells\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7E3A73B-9435-42EC-BF37-4599F635828A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3D33F6-B2C4-4856-B275-4DAB4DEC4BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>aa</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>merged rows</t>
-  </si>
-  <si>
-    <t>dd</t>
   </si>
   <si>
     <t>ee</t>
@@ -65,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -119,9 +116,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,7 +156,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -265,7 +262,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -407,18 +404,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -450,20 +447,17 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>